<commit_message>
Favourite widget is basically finished
</commit_message>
<xml_diff>
--- a/backend/default_images_and_spreadsheets/ItemsSample.xlsx
+++ b/backend/default_images_and_spreadsheets/ItemsSample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Python\PycharmProjects\belmarket\belmarket\default_images_and_spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Python\PycharmProjects\belmarket\belmarket\backend\default_images_and_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58B121F-C41B-45A5-ABA9-A75357F60724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C66B12-3E92-4B85-9E11-1110E35D217C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5412" yWindow="2988" windowWidth="12600" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Товары" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>Milk.jfif</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Just some beef</t>
+  </si>
+  <si>
+    <t>Test description for milk</t>
+  </si>
+  <si>
+    <t>Yoooo….. Ghurt.</t>
   </si>
 </sst>
 </file>
@@ -427,18 +439,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="13.109375" customWidth="1"/>
+    <col min="2" max="5" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,15 +458,17 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -463,8 +477,9 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -472,16 +487,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>600</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -489,16 +507,19 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>70</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -506,9 +527,12 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>50</v>
       </c>
     </row>

</xml_diff>